<commit_message>
Ajout de la création d'un csv
</commit_message>
<xml_diff>
--- a/FilesDIR_Data.xlsx
+++ b/FilesDIR_Data.xlsx
@@ -336,6 +336,9 @@
         <v>Date</v>
       </c>
       <c r="D1" t="str">
+        <v>Lien_Fichier</v>
+      </c>
+      <c r="E1" t="str">
         <v>Lien</v>
       </c>
     </row>
@@ -350,6 +353,9 @@
         <v>2022-03-30 21:54:29.8584158 +0200 CEST</v>
       </c>
       <c r="D2" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\13990489_014_32d5.jpg</v>
+      </c>
+      <c r="E2" t="str">
         <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
       </c>
     </row>
@@ -364,6 +370,9 @@
         <v>2022-03-30 20:20:08.377736 +0200 CEST</v>
       </c>
       <c r="D3" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\35521022_008_3818.jpg</v>
+      </c>
+      <c r="E3" t="str">
         <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
       </c>
     </row>
@@ -378,6 +387,9 @@
         <v>2022-03-30 20:20:16.8401081 +0200 CEST</v>
       </c>
       <c r="D4" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\42114357_008_e518.jpg</v>
+      </c>
+      <c r="E4" t="str">
         <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
       </c>
     </row>
@@ -392,6 +404,9 @@
         <v>2022-03-30 20:57:32.3231114 +0200 CEST</v>
       </c>
       <c r="D5" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\51264762_010_85fb.jpg</v>
+      </c>
+      <c r="E5" t="str">
         <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
       </c>
     </row>
@@ -406,6 +421,9 @@
         <v>2022-03-30 21:12:36.5423085 +0200 CEST</v>
       </c>
       <c r="D6" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\51668362_011_9509.jpg</v>
+      </c>
+      <c r="E6" t="str">
         <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
       </c>
     </row>
@@ -420,6 +438,9 @@
         <v>2022-03-30 20:20:25.5827521 +0200 CEST</v>
       </c>
       <c r="D7" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\53857573_012_4401.jpg</v>
+      </c>
+      <c r="E7" t="str">
         <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
       </c>
     </row>
@@ -434,6 +455,9 @@
         <v>2022-03-30 20:20:33.4386199 +0200 CEST</v>
       </c>
       <c r="D8" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\58988690_005_7337.jpg</v>
+      </c>
+      <c r="E8" t="str">
         <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
       </c>
     </row>
@@ -448,6 +472,9 @@
         <v>2022-03-30 21:29:56.5656533 +0200 CEST</v>
       </c>
       <c r="D9" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\61766583_004_0012.jpg</v>
+      </c>
+      <c r="E9" t="str">
         <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
       </c>
     </row>
@@ -462,6 +489,9 @@
         <v>2022-03-30 21:13:47.2499026 +0200 CEST</v>
       </c>
       <c r="D10" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\69008671_002_925b.jpg</v>
+      </c>
+      <c r="E10" t="str">
         <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
       </c>
     </row>
@@ -476,6 +506,9 @@
         <v>2022-03-30 20:20:47.9227773 +0200 CEST</v>
       </c>
       <c r="D11" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\86016225_008_7005.jpg</v>
+      </c>
+      <c r="E11" t="str">
         <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
       </c>
     </row>
@@ -490,6 +523,9 @@
         <v>2022-03-30 21:50:36.1524379 +0200 CEST</v>
       </c>
       <c r="D12" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\90282507_001_1a6b.jpg</v>
+      </c>
+      <c r="E12" t="str">
         <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
       </c>
     </row>
@@ -504,7 +540,10 @@
         <v>2022-03-30 22:00:36.292991 +0200 CEST</v>
       </c>
       <c r="D13" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\avantApres\18_1.jpg</v>
+      </c>
+      <c r="E13" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\avantApres</v>
       </c>
     </row>
     <row r="14">
@@ -518,7 +557,10 @@
         <v>2022-03-30 22:00:41.9629567 +0200 CEST</v>
       </c>
       <c r="D14" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\avantApres\18_2.jpg</v>
+      </c>
+      <c r="E14" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\avantApres</v>
       </c>
     </row>
     <row r="15">
@@ -532,7 +574,10 @@
         <v>2022-03-27 20:31:42.5479828 +0200 CEST</v>
       </c>
       <c r="D15" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\avantApres\8_1.jpg</v>
+      </c>
+      <c r="E15" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\avantApres</v>
       </c>
     </row>
     <row r="16">
@@ -546,7 +591,10 @@
         <v>2022-03-27 20:31:48.5672617 +0200 CEST</v>
       </c>
       <c r="D16" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\avantApres\8_2.jpg</v>
+      </c>
+      <c r="E16" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\avantApres</v>
       </c>
     </row>
     <row r="17">
@@ -560,7 +608,10 @@
         <v>2022-03-30 21:35:20.4719256 +0200 CEST</v>
       </c>
       <c r="D17" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bed\12781538_001_cca7.jpg</v>
+      </c>
+      <c r="E17" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bed</v>
       </c>
     </row>
     <row r="18">
@@ -574,7 +625,10 @@
         <v>2022-03-30 21:35:31.7153555 +0200 CEST</v>
       </c>
       <c r="D18" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bed\27648680_010_d49c.jpg</v>
+      </c>
+      <c r="E18" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bed</v>
       </c>
     </row>
     <row r="19">
@@ -588,7 +642,10 @@
         <v>2022-03-30 22:05:33.2026281 +0200 CEST</v>
       </c>
       <c r="D19" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bed\33800700_002_e076.jpg</v>
+      </c>
+      <c r="E19" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bed</v>
       </c>
     </row>
     <row r="20">
@@ -602,7 +659,10 @@
         <v>2022-03-30 21:35:37.2415781 +0200 CEST</v>
       </c>
       <c r="D20" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bed\58636886_005_5d44.jpg</v>
+      </c>
+      <c r="E20" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bed</v>
       </c>
     </row>
     <row r="21">
@@ -616,7 +676,10 @@
         <v>2022-03-30 21:35:54.5131233 +0200 CEST</v>
       </c>
       <c r="D21" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bed\59845869_003_97cb.jpg</v>
+      </c>
+      <c r="E21" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bed</v>
       </c>
     </row>
     <row r="22">
@@ -630,7 +693,10 @@
         <v>2022-03-30 20:13:49.2901201 +0200 CEST</v>
       </c>
       <c r="D22" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bed\68970141_011_c67c.jpg</v>
+      </c>
+      <c r="E22" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bed</v>
       </c>
     </row>
     <row r="23">
@@ -644,7 +710,10 @@
         <v>2022-03-30 21:43:43.8362887 +0200 CEST</v>
       </c>
       <c r="D23" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bed\70931302_002_0801.jpg</v>
+      </c>
+      <c r="E23" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bed</v>
       </c>
     </row>
     <row r="24">
@@ -658,7 +727,10 @@
         <v>2022-03-30 21:36:42.9733239 +0200 CEST</v>
       </c>
       <c r="D24" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bed\88695778_001_24e0.jpg</v>
+      </c>
+      <c r="E24" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bed</v>
       </c>
     </row>
     <row r="25">
@@ -672,7 +744,10 @@
         <v>2022-03-30 21:36:12.2732524 +0200 CEST</v>
       </c>
       <c r="D25" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bed\96615894_015_e0a7.jpg</v>
+      </c>
+      <c r="E25" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bed</v>
       </c>
     </row>
     <row r="26">
@@ -686,7 +761,10 @@
         <v>2022-03-30 20:14:02.9106994 +0200 CEST</v>
       </c>
       <c r="D26" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bikiniStreet\70689830_012_fafa.jpg</v>
+      </c>
+      <c r="E26" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bikiniStreet</v>
       </c>
     </row>
     <row r="27">
@@ -700,7 +778,10 @@
         <v>2022-03-05 21:27:41.8583915 +0100 CET</v>
       </c>
       <c r="D27" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bikiniStreet\jess-6zghg9yf56-1080x1348.jpg</v>
+      </c>
+      <c r="E27" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bikiniStreet</v>
       </c>
     </row>
     <row r="28">
@@ -714,7 +795,10 @@
         <v>2022-03-30 21:35:09.7705387 +0200 CEST</v>
       </c>
       <c r="D28" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\douche\32408092_003_5c4f.jpg</v>
+      </c>
+      <c r="E28" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\douche</v>
       </c>
     </row>
     <row r="29">
@@ -728,7 +812,10 @@
         <v>2022-03-30 20:14:22.2748096 +0200 CEST</v>
       </c>
       <c r="D29" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\douche\35383028_016_91d5.jpg</v>
+      </c>
+      <c r="E29" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\douche</v>
       </c>
     </row>
     <row r="30">
@@ -742,7 +829,10 @@
         <v>2022-03-15 20:32:48.411945 +0100 CET</v>
       </c>
       <c r="D30" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\douche\508914_10big.jpg</v>
+      </c>
+      <c r="E30" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\douche</v>
       </c>
     </row>
     <row r="31">
@@ -756,7 +846,10 @@
         <v>2022-03-15 20:33:05.6065958 +0100 CET</v>
       </c>
       <c r="D31" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\douche\single_003_1132101157082150.jpg</v>
+      </c>
+      <c r="E31" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\douche</v>
       </c>
     </row>
     <row r="32">
@@ -770,7 +863,10 @@
         <v>2022-03-30 20:14:54.4440483 +0200 CEST</v>
       </c>
       <c r="D32" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\doucheHabille\50061685_006_e80b.jpg</v>
+      </c>
+      <c r="E32" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\doucheHabille</v>
       </c>
     </row>
     <row r="33">
@@ -784,7 +880,10 @@
         <v>2022-03-30 20:15:13.9359267 +0200 CEST</v>
       </c>
       <c r="D33" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\gene\58314356_008_4c77.jpg</v>
+      </c>
+      <c r="E33" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\gene</v>
       </c>
     </row>
     <row r="34">
@@ -798,7 +897,10 @@
         <v>2022-03-30 20:15:26.9610981 +0200 CEST</v>
       </c>
       <c r="D34" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\innocent\39708365_005_5b3b.jpg</v>
+      </c>
+      <c r="E34" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\innocent</v>
       </c>
     </row>
     <row r="35">
@@ -812,7 +914,10 @@
         <v>2022-03-30 20:15:37.9296354 +0200 CEST</v>
       </c>
       <c r="D35" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\innocent\56640954_006_6287.jpg</v>
+      </c>
+      <c r="E35" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\innocent</v>
       </c>
     </row>
     <row r="36">
@@ -826,7 +931,10 @@
         <v>2022-03-30 20:16:07.0886658 +0200 CEST</v>
       </c>
       <c r="D36" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\irresistible\50061685_004_3421.jpg</v>
+      </c>
+      <c r="E36" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\irresistible</v>
       </c>
     </row>
     <row r="37">
@@ -840,7 +948,10 @@
         <v>2022-03-30 20:16:27.0921792 +0200 CEST</v>
       </c>
       <c r="D37" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\irresistible\60897441_004_4dcd.jpg</v>
+      </c>
+      <c r="E37" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\irresistible</v>
       </c>
     </row>
     <row r="38">
@@ -854,7 +965,10 @@
         <v>2022-03-30 20:16:35.7729663 +0200 CEST</v>
       </c>
       <c r="D38" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\irresistible\68802054_002_5de7.jpg</v>
+      </c>
+      <c r="E38" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\irresistible</v>
       </c>
     </row>
     <row r="39">
@@ -868,7 +982,10 @@
         <v>2022-03-30 21:51:18.3680014 +0200 CEST</v>
       </c>
       <c r="D39" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\irresistible\83172538_010_ab52.jpg</v>
+      </c>
+      <c r="E39" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\irresistible</v>
       </c>
     </row>
     <row r="40">
@@ -882,7 +999,10 @@
         <v>2022-03-19 19:05:07.4640105 +0100 CET</v>
       </c>
       <c r="D40" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\irresistible\960x1281_f55f0c6bf3bee310a7805f5c0fb8aa52.jpg</v>
+      </c>
+      <c r="E40" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\irresistible</v>
       </c>
     </row>
     <row r="41">
@@ -896,7 +1016,10 @@
         <v>2022-03-30 20:16:48.9247987 +0200 CEST</v>
       </c>
       <c r="D41" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\irresistible\ftv-girls-8.jpg</v>
+      </c>
+      <c r="E41" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\irresistible</v>
       </c>
     </row>
     <row r="42">
@@ -910,7 +1033,10 @@
         <v>2022-03-23 20:29:34.3215852 +0100 CET</v>
       </c>
       <c r="D42" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\irresistible\rosalina-in-treat-myself-by-matiss-18.jpg</v>
+      </c>
+      <c r="E42" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\irresistible</v>
       </c>
     </row>
     <row r="43">
@@ -924,7 +1050,10 @@
         <v>2022-03-19 19:56:42.9850117 +0100 CET</v>
       </c>
       <c r="D43" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\irresistible\yvnso02ycel81.png</v>
+      </c>
+      <c r="E43" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\irresistible</v>
       </c>
     </row>
     <row r="44">
@@ -938,7 +1067,10 @@
         <v>2021-12-27 20:51:40 +0100 CET</v>
       </c>
       <c r="D44" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\mainSeins\danifae_585.jpg</v>
+      </c>
+      <c r="E44" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\mainSeins</v>
       </c>
     </row>
     <row r="45">
@@ -952,7 +1084,10 @@
         <v>2022-03-30 21:33:46.743243 +0200 CEST</v>
       </c>
       <c r="D45" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\mousse\71861642_011_50ed.jpg</v>
+      </c>
+      <c r="E45" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\mousse</v>
       </c>
     </row>
     <row r="46">
@@ -966,7 +1101,10 @@
         <v>2022-03-05 20:58:27.9704985 +0100 CET</v>
       </c>
       <c r="D46" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\nuePro\0004-18.jpg</v>
+      </c>
+      <c r="E46" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\nuePro</v>
       </c>
     </row>
     <row r="47">
@@ -980,7 +1118,10 @@
         <v>2022-03-30 21:33:30.3202957 +0200 CEST</v>
       </c>
       <c r="D47" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\oops\20937858_005_ee65.jpg</v>
+      </c>
+      <c r="E47" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\oops</v>
       </c>
     </row>
     <row r="48">
@@ -994,7 +1135,10 @@
         <v>2022-03-30 20:17:32.1014521 +0200 CEST</v>
       </c>
       <c r="D48" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\oops\36717425_014_9837.jpg</v>
+      </c>
+      <c r="E48" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\oops</v>
       </c>
     </row>
     <row r="49">
@@ -1008,7 +1152,10 @@
         <v>2022-03-30 20:17:40.3912855 +0200 CEST</v>
       </c>
       <c r="D49" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\oops\71514153_015_8770.jpg</v>
+      </c>
+      <c r="E49" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\oops</v>
       </c>
     </row>
     <row r="50">
@@ -1022,7 +1169,10 @@
         <v>2022-03-30 20:17:47.6079888 +0200 CEST</v>
       </c>
       <c r="D50" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\oops\87527812_006_ad76.jpg</v>
+      </c>
+      <c r="E50" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\oops</v>
       </c>
     </row>
     <row r="51">
@@ -1036,7 +1186,10 @@
         <v>2022-03-30 20:17:56.0045365 +0200 CEST</v>
       </c>
       <c r="D51" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\oops\91294080_004_50ad.jpg</v>
+      </c>
+      <c r="E51" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\oops</v>
       </c>
     </row>
     <row r="52">
@@ -1050,7 +1203,10 @@
         <v>2022-03-19 21:14:42.8588295 +0100 CET</v>
       </c>
       <c r="D52" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\oops\960x1281_165ac01e6bb7389bd0913dac508a94d8.jpg</v>
+      </c>
+      <c r="E52" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\oops</v>
       </c>
     </row>
     <row r="53">
@@ -1064,7 +1220,10 @@
         <v>2021-12-27 20:51:40 +0100 CET</v>
       </c>
       <c r="D53" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\oops\danifae_589.jpg</v>
+      </c>
+      <c r="E53" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\oops</v>
       </c>
     </row>
     <row r="54">
@@ -1078,7 +1237,10 @@
         <v>2022-03-30 20:18:51.7236664 +0200 CEST</v>
       </c>
       <c r="D54" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\relaxed\36855676_016_5542.jpg</v>
+      </c>
+      <c r="E54" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\relaxed</v>
       </c>
     </row>
     <row r="55">
@@ -1092,7 +1254,10 @@
         <v>2022-03-30 20:19:04.5194511 +0200 CEST</v>
       </c>
       <c r="D55" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\relaxed\71684139_009_8528.jpg</v>
+      </c>
+      <c r="E55" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\relaxed</v>
       </c>
     </row>
     <row r="56">
@@ -1106,7 +1271,10 @@
         <v>2022-03-05 21:31:35.3435616 +0100 CET</v>
       </c>
       <c r="D56" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sexyNoNude\harlee-c5aqpmd49h-1078x1350.jpg</v>
+      </c>
+      <c r="E56" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sexyNoNude</v>
       </c>
     </row>
     <row r="57">
@@ -1120,7 +1288,10 @@
         <v>2022-03-05 21:26:05.6187394 +0100 CET</v>
       </c>
       <c r="D57" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sexyNoNude\in-the-right-spot-7tnmucsxwi-1080x1115.jpg</v>
+      </c>
+      <c r="E57" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sexyNoNude</v>
       </c>
     </row>
     <row r="58">
@@ -1134,7 +1305,10 @@
         <v>2022-03-05 21:36:39.8037549 +0100 CET</v>
       </c>
       <c r="D58" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sexyNoNude\just-perfect-imtxhvbo7h-1080x1345.jpg</v>
+      </c>
+      <c r="E58" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sexyNoNude</v>
       </c>
     </row>
     <row r="59">
@@ -1148,7 +1322,10 @@
         <v>2022-03-05 21:28:26.6143293 +0100 CET</v>
       </c>
       <c r="D59" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sexyNoNude\lara-aek604owoe-1078x1350.jpg</v>
+      </c>
+      <c r="E59" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sexyNoNude</v>
       </c>
     </row>
     <row r="60">
@@ -1162,7 +1339,10 @@
         <v>2022-03-05 21:38:46.166225 +0100 CET</v>
       </c>
       <c r="D60" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sexyNoNude\untitled-bbsarowjsk-1080x1350.jpg</v>
+      </c>
+      <c r="E60" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sexyNoNude</v>
       </c>
     </row>
     <row r="61">
@@ -1176,7 +1356,10 @@
         <v>2022-03-09 21:23:58.2896457 +0100 CET</v>
       </c>
       <c r="D61" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sortirDouche\3024x4032_5a1f6ca23e801d342af50473a1ff2c39.jpg</v>
+      </c>
+      <c r="E61" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sortirDouche</v>
       </c>
     </row>
     <row r="62">
@@ -1190,7 +1373,10 @@
         <v>2022-03-30 21:32:55.187877 +0200 CEST</v>
       </c>
       <c r="D62" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sortirDouche\32408092_012_5ad4.jpg</v>
+      </c>
+      <c r="E62" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sortirDouche</v>
       </c>
     </row>
     <row r="63">
@@ -1204,7 +1390,10 @@
         <v>2022-03-09 20:52:25.5926621 +0100 CET</v>
       </c>
       <c r="D63" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sortirDouche\89920516_016_5d4f.jpg</v>
+      </c>
+      <c r="E63" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sortirDouche</v>
       </c>
     </row>
     <row r="64">
@@ -1218,7 +1407,10 @@
         <v>2022-03-09 21:21:58.9703899 +0100 CET</v>
       </c>
       <c r="D64" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sortirDouche\960x2079_d89c4f160b2dd28e0da5482c79653091.jpg</v>
+      </c>
+      <c r="E64" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sortirDouche</v>
       </c>
     </row>
     <row r="65">
@@ -1232,7 +1424,10 @@
         <v>2021-12-27 20:51:40 +0100 CET</v>
       </c>
       <c r="D65" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sortirDouche\danifae_1488.jpg</v>
+      </c>
+      <c r="E65" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sortirDouche</v>
       </c>
     </row>
     <row r="66">
@@ -1246,7 +1441,10 @@
         <v>2022-03-09 21:09:57.1381803 +0100 CET</v>
       </c>
       <c r="D66" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sortirDouche\would-i-make-you-hard-if-i-sent-you-shower-nudes-boiq95qes1-1080x1440.jpg</v>
+      </c>
+      <c r="E66" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sortirDouche</v>
       </c>
     </row>
     <row r="67">
@@ -1260,7 +1458,10 @@
         <v>2022-03-30 21:33:14.8811013 +0200 CEST</v>
       </c>
       <c r="D67" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\towel\95833571_001_173d.jpg</v>
+      </c>
+      <c r="E67" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\towel</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout de la création d'un json
</commit_message>
<xml_diff>
--- a/FilesDIR_Data.xlsx
+++ b/FilesDIR_Data.xlsx
@@ -342,72 +342,40 @@
         <v>Lien</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="str">
-        <v>&amp;éàÉ@.jpg</v>
-      </c>
-      <c r="C2" t="str">
-        <v>2022-03-30 20:20:47.9227773 +0200 CEST</v>
-      </c>
-      <c r="D2" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux\fddddddddddàç&amp;éÉddddddd\&amp;éàÉ@.jpg</v>
-      </c>
-      <c r="E2" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux\fddddddddddàç&amp;éÉddddddd</v>
-      </c>
-    </row>
+    <row r="2"/>
     <row r="3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="str">
-        <v>02.jpg</v>
+        <v>13990489_014_32d5.jpg</v>
       </c>
       <c r="C3" t="str">
-        <v>2022-03-30 20:20:00.837897 +0200 CEST</v>
+        <v>2022-03-30 21:54:29.8584158 +0200 CEST</v>
       </c>
       <c r="D3" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux\fddddddddddàç&amp;éÉddddddd\02.jpg</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\13990489_014_32d5.jpg</v>
       </c>
       <c r="E3" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux\fddddddddddàç&amp;éÉddddddd</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="str">
-        <v>13990489_014_32d5.jpg</v>
-      </c>
-      <c r="C4" t="str">
-        <v>2022-03-30 21:54:29.8584158 +0200 CEST</v>
-      </c>
-      <c r="D4" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux\fddddddddddàç&amp;éÉddddddd\13990489_014_32d5.jpg</v>
-      </c>
-      <c r="E4" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux\fddddddddddàç&amp;éÉddddddd</v>
-      </c>
-    </row>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+      </c>
+    </row>
+    <row r="4"/>
     <row r="5">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="str">
-        <v>2.jpg</v>
+        <v>35521022_008_3818.jpg</v>
       </c>
       <c r="C5" t="str">
-        <v>2022-03-23 20:30:49.2668034 +0100 CET</v>
+        <v>2022-03-30 20:20:08.377736 +0200 CEST</v>
       </c>
       <c r="D5" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux\fddddddddddàç&amp;éÉddddddd\2.jpg</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\35521022_008_3818.jpg</v>
       </c>
       <c r="E5" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux\fddddddddddàç&amp;éÉddddddd</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
       </c>
     </row>
     <row r="6">
@@ -415,16 +383,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="str">
-        <v>58988690_005_7337 - Copie.jpg</v>
+        <v>42114357_008_e518.jpg</v>
       </c>
       <c r="C6" t="str">
-        <v>2022-03-30 20:20:33.4386199 +0200 CEST</v>
+        <v>2022-03-30 20:20:16.8401081 +0200 CEST</v>
       </c>
       <c r="D6" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux\fddddddddddàç&amp;éÉddddddd\58988690_005_7337 - Copie.jpg</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\42114357_008_e518.jpg</v>
       </c>
       <c r="E6" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux\fddddddddddàç&amp;éÉddddddd</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
       </c>
     </row>
     <row r="7">
@@ -432,16 +400,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="str">
-        <v>58988690_fffffffffffff.jpg</v>
+        <v>51264762_010_85fb.jpg</v>
       </c>
       <c r="C7" t="str">
-        <v>2022-03-30 20:20:33.4386199 +0200 CEST</v>
+        <v>2022-03-30 20:57:32.3231114 +0200 CEST</v>
       </c>
       <c r="D7" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux\fddddddddddàç&amp;éÉddddddd\58988690_fffffffffffff.jpg</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\51264762_010_85fb.jpg</v>
       </c>
       <c r="E7" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux\fddddddddddàç&amp;éÉddddddd</v>
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
       </c>
     </row>
     <row r="8">
@@ -449,16 +417,1151 @@
         <v>7</v>
       </c>
       <c r="B8" t="str">
-        <v>danifae_1255 - Copie èèéé.jpg</v>
+        <v>51668362_011_9509.jpg</v>
       </c>
       <c r="C8" t="str">
+        <v>2022-03-30 21:12:36.5423085 +0200 CEST</v>
+      </c>
+      <c r="D8" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\51668362_011_9509.jpg</v>
+      </c>
+      <c r="E8" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="str">
+        <v>53857573_012_4401.jpg</v>
+      </c>
+      <c r="C9" t="str">
+        <v>2022-03-30 20:20:25.5827521 +0200 CEST</v>
+      </c>
+      <c r="D9" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\53857573_012_4401.jpg</v>
+      </c>
+      <c r="E9" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="str">
+        <v>58988690_005_7337.jpg</v>
+      </c>
+      <c r="C10" t="str">
+        <v>2022-03-30 20:20:33.4386199 +0200 CEST</v>
+      </c>
+      <c r="D10" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\58988690_005_7337.jpg</v>
+      </c>
+      <c r="E10" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="str">
+        <v>61766583_004_0012.jpg</v>
+      </c>
+      <c r="C11" t="str">
+        <v>2022-03-30 21:29:56.5656533 +0200 CEST</v>
+      </c>
+      <c r="D11" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\61766583_004_0012.jpg</v>
+      </c>
+      <c r="E11" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+      </c>
+    </row>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="str">
+        <v>69008671_002_925b.jpg</v>
+      </c>
+      <c r="C14" t="str">
+        <v>2022-03-30 21:13:47.2499026 +0200 CEST</v>
+      </c>
+      <c r="D14" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\69008671_002_925b.jpg</v>
+      </c>
+      <c r="E14" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+      </c>
+    </row>
+    <row r="15"/>
+    <row r="16">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="str">
+        <v>86016225_008_7005.jpg</v>
+      </c>
+      <c r="C16" t="str">
+        <v>2022-03-30 20:20:47.9227773 +0200 CEST</v>
+      </c>
+      <c r="D16" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\86016225_008_7005.jpg</v>
+      </c>
+      <c r="E16" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="str">
+        <v>90282507_001_1a6b.jpg</v>
+      </c>
+      <c r="C17" t="str">
+        <v>2022-03-30 21:50:36.1524379 +0200 CEST</v>
+      </c>
+      <c r="D17" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\90282507_001_1a6b.jpg</v>
+      </c>
+      <c r="E17" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux</v>
+      </c>
+    </row>
+    <row r="18"/>
+    <row r="19"/>
+    <row r="20"/>
+    <row r="21"/>
+    <row r="22"/>
+    <row r="23"/>
+    <row r="24"/>
+    <row r="25"/>
+    <row r="26"/>
+    <row r="27"/>
+    <row r="28"/>
+    <row r="29"/>
+    <row r="30"/>
+    <row r="31"/>
+    <row r="32"/>
+    <row r="33"/>
+    <row r="34">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="str">
+        <v>18_1.jpg</v>
+      </c>
+      <c r="C34" t="str">
+        <v>2022-03-30 22:00:36.292991 +0200 CEST</v>
+      </c>
+      <c r="D34" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\avantApres\18_1.jpg</v>
+      </c>
+      <c r="E34" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\avantApres</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="str">
+        <v>18_2.jpg</v>
+      </c>
+      <c r="C35" t="str">
+        <v>2022-03-30 22:00:41.9629567 +0200 CEST</v>
+      </c>
+      <c r="D35" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\avantApres\18_2.jpg</v>
+      </c>
+      <c r="E35" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\avantApres</v>
+      </c>
+    </row>
+    <row r="36"/>
+    <row r="37"/>
+    <row r="38"/>
+    <row r="39"/>
+    <row r="40"/>
+    <row r="41"/>
+    <row r="42"/>
+    <row r="43"/>
+    <row r="44"/>
+    <row r="45"/>
+    <row r="46"/>
+    <row r="47"/>
+    <row r="48"/>
+    <row r="49"/>
+    <row r="50"/>
+    <row r="51"/>
+    <row r="52"/>
+    <row r="53"/>
+    <row r="54"/>
+    <row r="55"/>
+    <row r="56">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="str">
+        <v>8_1.jpg</v>
+      </c>
+      <c r="C56" t="str">
+        <v>2022-03-27 20:31:42.5479828 +0200 CEST</v>
+      </c>
+      <c r="D56" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\avantApres\8_1.jpg</v>
+      </c>
+      <c r="E56" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\avantApres</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="str">
+        <v>8_2.jpg</v>
+      </c>
+      <c r="C57" t="str">
+        <v>2022-03-27 20:31:48.5672617 +0200 CEST</v>
+      </c>
+      <c r="D57" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\avantApres\8_2.jpg</v>
+      </c>
+      <c r="E57" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\avantApres</v>
+      </c>
+    </row>
+    <row r="58"/>
+    <row r="59"/>
+    <row r="60">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="str">
+        <v>12781538_001_cca7.jpg</v>
+      </c>
+      <c r="C60" t="str">
+        <v>2022-03-30 21:35:20.4719256 +0200 CEST</v>
+      </c>
+      <c r="D60" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bed\12781538_001_cca7.jpg</v>
+      </c>
+      <c r="E60" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bed</v>
+      </c>
+    </row>
+    <row r="61"/>
+    <row r="62">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="str">
+        <v>27648680_010_d49c.jpg</v>
+      </c>
+      <c r="C62" t="str">
+        <v>2022-03-30 21:35:31.7153555 +0200 CEST</v>
+      </c>
+      <c r="D62" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bed\27648680_010_d49c.jpg</v>
+      </c>
+      <c r="E62" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bed</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="str">
+        <v>33800700_002_e076.jpg</v>
+      </c>
+      <c r="C63" t="str">
+        <v>2022-03-30 22:05:33.2026281 +0200 CEST</v>
+      </c>
+      <c r="D63" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bed\33800700_002_e076.jpg</v>
+      </c>
+      <c r="E63" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bed</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="str">
+        <v>58636886_005_5d44.jpg</v>
+      </c>
+      <c r="C64" t="str">
+        <v>2022-03-30 21:35:37.2415781 +0200 CEST</v>
+      </c>
+      <c r="D64" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bed\58636886_005_5d44.jpg</v>
+      </c>
+      <c r="E64" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bed</v>
+      </c>
+    </row>
+    <row r="65"/>
+    <row r="66">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="str">
+        <v>59845869_003_97cb.jpg</v>
+      </c>
+      <c r="C66" t="str">
+        <v>2022-03-30 21:35:54.5131233 +0200 CEST</v>
+      </c>
+      <c r="D66" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bed\59845869_003_97cb.jpg</v>
+      </c>
+      <c r="E66" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bed</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="str">
+        <v>68970141_011_c67c.jpg</v>
+      </c>
+      <c r="C67" t="str">
+        <v>2022-03-30 20:13:49.2901201 +0200 CEST</v>
+      </c>
+      <c r="D67" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bed\68970141_011_c67c.jpg</v>
+      </c>
+      <c r="E67" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bed</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="str">
+        <v>70931302_002_0801.jpg</v>
+      </c>
+      <c r="C68" t="str">
+        <v>2022-03-30 21:43:43.8362887 +0200 CEST</v>
+      </c>
+      <c r="D68" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bed\70931302_002_0801.jpg</v>
+      </c>
+      <c r="E68" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bed</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" t="str">
+        <v>88695778_001_24e0.jpg</v>
+      </c>
+      <c r="C69" t="str">
+        <v>2022-03-30 21:36:42.9733239 +0200 CEST</v>
+      </c>
+      <c r="D69" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bed\88695778_001_24e0.jpg</v>
+      </c>
+      <c r="E69" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bed</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="str">
+        <v>96615894_015_e0a7.jpg</v>
+      </c>
+      <c r="C70" t="str">
+        <v>2022-03-30 21:36:12.2732524 +0200 CEST</v>
+      </c>
+      <c r="D70" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bed\96615894_015_e0a7.jpg</v>
+      </c>
+      <c r="E70" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bed</v>
+      </c>
+    </row>
+    <row r="71"/>
+    <row r="72">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" t="str">
+        <v>70689830_012_fafa.jpg</v>
+      </c>
+      <c r="C72" t="str">
+        <v>2022-03-30 20:14:02.9106994 +0200 CEST</v>
+      </c>
+      <c r="D72" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bikiniStreet\70689830_012_fafa.jpg</v>
+      </c>
+      <c r="E72" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bikiniStreet</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" t="str">
+        <v>jess-6zghg9yf56-1080x1348.jpg</v>
+      </c>
+      <c r="C73" t="str">
+        <v>2022-03-05 21:27:41.8583915 +0100 CET</v>
+      </c>
+      <c r="D73" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bikiniStreet\jess-6zghg9yf56-1080x1348.jpg</v>
+      </c>
+      <c r="E73" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\bikiniStreet</v>
+      </c>
+    </row>
+    <row r="74"/>
+    <row r="75"/>
+    <row r="76"/>
+    <row r="77"/>
+    <row r="78">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" t="str">
+        <v>32408092_003_5c4f.jpg</v>
+      </c>
+      <c r="C78" t="str">
+        <v>2022-03-30 21:35:09.7705387 +0200 CEST</v>
+      </c>
+      <c r="D78" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\douche\32408092_003_5c4f.jpg</v>
+      </c>
+      <c r="E78" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\douche</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" t="str">
+        <v>35383028_016_91d5.jpg</v>
+      </c>
+      <c r="C79" t="str">
+        <v>2022-03-30 20:14:22.2748096 +0200 CEST</v>
+      </c>
+      <c r="D79" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\douche\35383028_016_91d5.jpg</v>
+      </c>
+      <c r="E79" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\douche</v>
+      </c>
+    </row>
+    <row r="80"/>
+    <row r="81">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" t="str">
+        <v>508914_10big.jpg</v>
+      </c>
+      <c r="C81" t="str">
+        <v>2022-03-15 20:32:48.411945 +0100 CET</v>
+      </c>
+      <c r="D81" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\douche\508914_10big.jpg</v>
+      </c>
+      <c r="E81" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\douche</v>
+      </c>
+    </row>
+    <row r="82"/>
+    <row r="83"/>
+    <row r="84">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84" t="str">
+        <v>single_003_1132101157082150.jpg</v>
+      </c>
+      <c r="C84" t="str">
+        <v>2022-03-15 20:33:05.6065958 +0100 CET</v>
+      </c>
+      <c r="D84" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\douche\single_003_1132101157082150.jpg</v>
+      </c>
+      <c r="E84" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\douche</v>
+      </c>
+    </row>
+    <row r="85"/>
+    <row r="86"/>
+    <row r="87"/>
+    <row r="88"/>
+    <row r="89">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89" t="str">
+        <v>50061685_006_e80b.jpg</v>
+      </c>
+      <c r="C89" t="str">
+        <v>2022-03-30 20:14:54.4440483 +0200 CEST</v>
+      </c>
+      <c r="D89" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\doucheHabille\50061685_006_e80b.jpg</v>
+      </c>
+      <c r="E89" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\doucheHabille</v>
+      </c>
+    </row>
+    <row r="90"/>
+    <row r="91"/>
+    <row r="92"/>
+    <row r="93">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93" t="str">
+        <v>58314356_008_4c77.jpg</v>
+      </c>
+      <c r="C93" t="str">
+        <v>2022-03-30 20:15:13.9359267 +0200 CEST</v>
+      </c>
+      <c r="D93" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\gene\58314356_008_4c77.jpg</v>
+      </c>
+      <c r="E93" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\gene</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94" t="str">
+        <v>39708365_005_5b3b.jpg</v>
+      </c>
+      <c r="C94" t="str">
+        <v>2022-03-30 20:15:26.9610981 +0200 CEST</v>
+      </c>
+      <c r="D94" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\innocent\39708365_005_5b3b.jpg</v>
+      </c>
+      <c r="E94" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\innocent</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95" t="str">
+        <v>56640954_006_6287.jpg</v>
+      </c>
+      <c r="C95" t="str">
+        <v>2022-03-30 20:15:37.9296354 +0200 CEST</v>
+      </c>
+      <c r="D95" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\innocent\56640954_006_6287.jpg</v>
+      </c>
+      <c r="E95" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\innocent</v>
+      </c>
+    </row>
+    <row r="96"/>
+    <row r="97"/>
+    <row r="98"/>
+    <row r="99"/>
+    <row r="100">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100" t="str">
+        <v>50061685_004_3421.jpg</v>
+      </c>
+      <c r="C100" t="str">
+        <v>2022-03-30 20:16:07.0886658 +0200 CEST</v>
+      </c>
+      <c r="D100" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\irresistible\50061685_004_3421.jpg</v>
+      </c>
+      <c r="E100" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\irresistible</v>
+      </c>
+    </row>
+    <row r="101"/>
+    <row r="102"/>
+    <row r="103">
+      <c r="A103">
+        <v>102</v>
+      </c>
+      <c r="B103" t="str">
+        <v>60897441_004_4dcd.jpg</v>
+      </c>
+      <c r="C103" t="str">
+        <v>2022-03-30 20:16:27.0921792 +0200 CEST</v>
+      </c>
+      <c r="D103" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\irresistible\60897441_004_4dcd.jpg</v>
+      </c>
+      <c r="E103" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\irresistible</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104">
+        <v>103</v>
+      </c>
+      <c r="B104" t="str">
+        <v>68802054_002_5de7.jpg</v>
+      </c>
+      <c r="C104" t="str">
+        <v>2022-03-30 20:16:35.7729663 +0200 CEST</v>
+      </c>
+      <c r="D104" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\irresistible\68802054_002_5de7.jpg</v>
+      </c>
+      <c r="E104" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\irresistible</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105">
+        <v>104</v>
+      </c>
+      <c r="B105" t="str">
+        <v>83172538_010_ab52.jpg</v>
+      </c>
+      <c r="C105" t="str">
+        <v>2022-03-30 21:51:18.3680014 +0200 CEST</v>
+      </c>
+      <c r="D105" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\irresistible\83172538_010_ab52.jpg</v>
+      </c>
+      <c r="E105" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\irresistible</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106">
+        <v>105</v>
+      </c>
+      <c r="B106" t="str">
+        <v>960x1281_f55f0c6bf3bee310a7805f5c0fb8aa52.jpg</v>
+      </c>
+      <c r="C106" t="str">
+        <v>2022-03-19 19:05:07.4640105 +0100 CET</v>
+      </c>
+      <c r="D106" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\irresistible\960x1281_f55f0c6bf3bee310a7805f5c0fb8aa52.jpg</v>
+      </c>
+      <c r="E106" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\irresistible</v>
+      </c>
+    </row>
+    <row r="107"/>
+    <row r="108"/>
+    <row r="109"/>
+    <row r="110"/>
+    <row r="111"/>
+    <row r="112"/>
+    <row r="113">
+      <c r="A113">
+        <v>112</v>
+      </c>
+      <c r="B113" t="str">
+        <v>ftv-girls-8.jpg</v>
+      </c>
+      <c r="C113" t="str">
+        <v>2022-03-30 20:16:48.9247987 +0200 CEST</v>
+      </c>
+      <c r="D113" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\irresistible\ftv-girls-8.jpg</v>
+      </c>
+      <c r="E113" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\irresistible</v>
+      </c>
+    </row>
+    <row r="114"/>
+    <row r="115"/>
+    <row r="116">
+      <c r="A116">
+        <v>115</v>
+      </c>
+      <c r="B116" t="str">
+        <v>rosalina-in-treat-myself-by-matiss-18.jpg</v>
+      </c>
+      <c r="C116" t="str">
+        <v>2022-03-23 20:29:34.3215852 +0100 CET</v>
+      </c>
+      <c r="D116" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\irresistible\rosalina-in-treat-myself-by-matiss-18.jpg</v>
+      </c>
+      <c r="E116" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\irresistible</v>
+      </c>
+    </row>
+    <row r="117"/>
+    <row r="118">
+      <c r="A118">
+        <v>117</v>
+      </c>
+      <c r="B118" t="str">
+        <v>yvnso02ycel81.png</v>
+      </c>
+      <c r="C118" t="str">
+        <v>2022-03-19 19:56:42.9850117 +0100 CET</v>
+      </c>
+      <c r="D118" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\irresistible\yvnso02ycel81.png</v>
+      </c>
+      <c r="E118" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\irresistible</v>
+      </c>
+    </row>
+    <row r="119"/>
+    <row r="120"/>
+    <row r="121">
+      <c r="A121">
+        <v>120</v>
+      </c>
+      <c r="B121" t="str">
+        <v>danifae_585.jpg</v>
+      </c>
+      <c r="C121" t="str">
         <v>2021-12-27 20:51:40 +0100 CET</v>
       </c>
-      <c r="D8" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux\fddddddddddàç&amp;éÉddddddd\danifae_1255 - Copie èèéé.jpg</v>
-      </c>
-      <c r="E8" t="str">
-        <v>F:\testBis\dl\Nouveau dossier\_Jeux\fddddddddddàç&amp;éÉddddddd</v>
+      <c r="D121" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\mainSeins\danifae_585.jpg</v>
+      </c>
+      <c r="E121" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\mainSeins</v>
+      </c>
+    </row>
+    <row r="122"/>
+    <row r="123"/>
+    <row r="124">
+      <c r="A124">
+        <v>123</v>
+      </c>
+      <c r="B124" t="str">
+        <v>71861642_011_50ed.jpg</v>
+      </c>
+      <c r="C124" t="str">
+        <v>2022-03-30 21:33:46.743243 +0200 CEST</v>
+      </c>
+      <c r="D124" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\mousse\71861642_011_50ed.jpg</v>
+      </c>
+      <c r="E124" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\mousse</v>
+      </c>
+    </row>
+    <row r="125"/>
+    <row r="126">
+      <c r="A126">
+        <v>125</v>
+      </c>
+      <c r="B126" t="str">
+        <v>0004-18.jpg</v>
+      </c>
+      <c r="C126" t="str">
+        <v>2022-03-05 20:58:27.9704985 +0100 CET</v>
+      </c>
+      <c r="D126" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\nuePro\0004-18.jpg</v>
+      </c>
+      <c r="E126" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\nuePro</v>
+      </c>
+    </row>
+    <row r="127"/>
+    <row r="128"/>
+    <row r="129">
+      <c r="A129">
+        <v>128</v>
+      </c>
+      <c r="B129" t="str">
+        <v>20937858_005_ee65.jpg</v>
+      </c>
+      <c r="C129" t="str">
+        <v>2022-03-30 21:33:30.3202957 +0200 CEST</v>
+      </c>
+      <c r="D129" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\oops\20937858_005_ee65.jpg</v>
+      </c>
+      <c r="E129" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\oops</v>
+      </c>
+    </row>
+    <row r="130"/>
+    <row r="131">
+      <c r="A131">
+        <v>130</v>
+      </c>
+      <c r="B131" t="str">
+        <v>36717425_014_9837.jpg</v>
+      </c>
+      <c r="C131" t="str">
+        <v>2022-03-30 20:17:32.1014521 +0200 CEST</v>
+      </c>
+      <c r="D131" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\oops\36717425_014_9837.jpg</v>
+      </c>
+      <c r="E131" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\oops</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132">
+        <v>131</v>
+      </c>
+      <c r="B132" t="str">
+        <v>71514153_015_8770.jpg</v>
+      </c>
+      <c r="C132" t="str">
+        <v>2022-03-30 20:17:40.3912855 +0200 CEST</v>
+      </c>
+      <c r="D132" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\oops\71514153_015_8770.jpg</v>
+      </c>
+      <c r="E132" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\oops</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133">
+        <v>132</v>
+      </c>
+      <c r="B133" t="str">
+        <v>87527812_006_ad76.jpg</v>
+      </c>
+      <c r="C133" t="str">
+        <v>2022-03-30 20:17:47.6079888 +0200 CEST</v>
+      </c>
+      <c r="D133" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\oops\87527812_006_ad76.jpg</v>
+      </c>
+      <c r="E133" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\oops</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134">
+        <v>133</v>
+      </c>
+      <c r="B134" t="str">
+        <v>91294080_004_50ad.jpg</v>
+      </c>
+      <c r="C134" t="str">
+        <v>2022-03-30 20:17:56.0045365 +0200 CEST</v>
+      </c>
+      <c r="D134" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\oops\91294080_004_50ad.jpg</v>
+      </c>
+      <c r="E134" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\oops</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135">
+        <v>134</v>
+      </c>
+      <c r="B135" t="str">
+        <v>960x1281_165ac01e6bb7389bd0913dac508a94d8.jpg</v>
+      </c>
+      <c r="C135" t="str">
+        <v>2022-03-19 21:14:42.8588295 +0100 CET</v>
+      </c>
+      <c r="D135" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\oops\960x1281_165ac01e6bb7389bd0913dac508a94d8.jpg</v>
+      </c>
+      <c r="E135" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\oops</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136">
+        <v>135</v>
+      </c>
+      <c r="B136" t="str">
+        <v>danifae_589.jpg</v>
+      </c>
+      <c r="C136" t="str">
+        <v>2021-12-27 20:51:40 +0100 CET</v>
+      </c>
+      <c r="D136" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\oops\danifae_589.jpg</v>
+      </c>
+      <c r="E136" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\oops</v>
+      </c>
+    </row>
+    <row r="137"/>
+    <row r="138"/>
+    <row r="139"/>
+    <row r="140"/>
+    <row r="141"/>
+    <row r="142"/>
+    <row r="143">
+      <c r="A143">
+        <v>142</v>
+      </c>
+      <c r="B143" t="str">
+        <v>36855676_016_5542.jpg</v>
+      </c>
+      <c r="C143" t="str">
+        <v>2022-03-30 20:18:51.7236664 +0200 CEST</v>
+      </c>
+      <c r="D143" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\relaxed\36855676_016_5542.jpg</v>
+      </c>
+      <c r="E143" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\relaxed</v>
+      </c>
+    </row>
+    <row r="144"/>
+    <row r="145">
+      <c r="A145">
+        <v>144</v>
+      </c>
+      <c r="B145" t="str">
+        <v>71684139_009_8528.jpg</v>
+      </c>
+      <c r="C145" t="str">
+        <v>2022-03-30 20:19:04.5194511 +0200 CEST</v>
+      </c>
+      <c r="D145" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\relaxed\71684139_009_8528.jpg</v>
+      </c>
+      <c r="E145" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\relaxed</v>
+      </c>
+    </row>
+    <row r="146"/>
+    <row r="147"/>
+    <row r="148"/>
+    <row r="149">
+      <c r="A149">
+        <v>148</v>
+      </c>
+      <c r="B149" t="str">
+        <v>harlee-c5aqpmd49h-1078x1350.jpg</v>
+      </c>
+      <c r="C149" t="str">
+        <v>2022-03-05 21:31:35.3435616 +0100 CET</v>
+      </c>
+      <c r="D149" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sexyNoNude\harlee-c5aqpmd49h-1078x1350.jpg</v>
+      </c>
+      <c r="E149" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sexyNoNude</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150">
+        <v>149</v>
+      </c>
+      <c r="B150" t="str">
+        <v>in-the-right-spot-7tnmucsxwi-1080x1115.jpg</v>
+      </c>
+      <c r="C150" t="str">
+        <v>2022-03-05 21:26:05.6187394 +0100 CET</v>
+      </c>
+      <c r="D150" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sexyNoNude\in-the-right-spot-7tnmucsxwi-1080x1115.jpg</v>
+      </c>
+      <c r="E150" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sexyNoNude</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151">
+        <v>150</v>
+      </c>
+      <c r="B151" t="str">
+        <v>just-perfect-imtxhvbo7h-1080x1345.jpg</v>
+      </c>
+      <c r="C151" t="str">
+        <v>2022-03-05 21:36:39.8037549 +0100 CET</v>
+      </c>
+      <c r="D151" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sexyNoNude\just-perfect-imtxhvbo7h-1080x1345.jpg</v>
+      </c>
+      <c r="E151" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sexyNoNude</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152">
+        <v>151</v>
+      </c>
+      <c r="B152" t="str">
+        <v>lara-aek604owoe-1078x1350.jpg</v>
+      </c>
+      <c r="C152" t="str">
+        <v>2022-03-05 21:28:26.6143293 +0100 CET</v>
+      </c>
+      <c r="D152" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sexyNoNude\lara-aek604owoe-1078x1350.jpg</v>
+      </c>
+      <c r="E152" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sexyNoNude</v>
+      </c>
+    </row>
+    <row r="153"/>
+    <row r="154"/>
+    <row r="155">
+      <c r="A155">
+        <v>154</v>
+      </c>
+      <c r="B155" t="str">
+        <v>untitled-bbsarowjsk-1080x1350.jpg</v>
+      </c>
+      <c r="C155" t="str">
+        <v>2022-03-05 21:38:46.166225 +0100 CET</v>
+      </c>
+      <c r="D155" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sexyNoNude\untitled-bbsarowjsk-1080x1350.jpg</v>
+      </c>
+      <c r="E155" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sexyNoNude</v>
+      </c>
+    </row>
+    <row r="156"/>
+    <row r="157">
+      <c r="A157">
+        <v>156</v>
+      </c>
+      <c r="B157" t="str">
+        <v>3024x4032_5a1f6ca23e801d342af50473a1ff2c39.jpg</v>
+      </c>
+      <c r="C157" t="str">
+        <v>2022-03-09 21:23:58.2896457 +0100 CET</v>
+      </c>
+      <c r="D157" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sortirDouche\3024x4032_5a1f6ca23e801d342af50473a1ff2c39.jpg</v>
+      </c>
+      <c r="E157" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sortirDouche</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158">
+        <v>157</v>
+      </c>
+      <c r="B158" t="str">
+        <v>32408092_012_5ad4.jpg</v>
+      </c>
+      <c r="C158" t="str">
+        <v>2022-03-30 21:32:55.187877 +0200 CEST</v>
+      </c>
+      <c r="D158" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sortirDouche\32408092_012_5ad4.jpg</v>
+      </c>
+      <c r="E158" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sortirDouche</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159">
+        <v>158</v>
+      </c>
+      <c r="B159" t="str">
+        <v>89920516_016_5d4f.jpg</v>
+      </c>
+      <c r="C159" t="str">
+        <v>2022-03-09 20:52:25.5926621 +0100 CET</v>
+      </c>
+      <c r="D159" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sortirDouche\89920516_016_5d4f.jpg</v>
+      </c>
+      <c r="E159" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sortirDouche</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160">
+        <v>159</v>
+      </c>
+      <c r="B160" t="str">
+        <v>960x2079_d89c4f160b2dd28e0da5482c79653091.jpg</v>
+      </c>
+      <c r="C160" t="str">
+        <v>2022-03-09 21:21:58.9703899 +0100 CET</v>
+      </c>
+      <c r="D160" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sortirDouche\960x2079_d89c4f160b2dd28e0da5482c79653091.jpg</v>
+      </c>
+      <c r="E160" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sortirDouche</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161">
+        <v>160</v>
+      </c>
+      <c r="B161" t="str">
+        <v>danifae_1488.jpg</v>
+      </c>
+      <c r="C161" t="str">
+        <v>2021-12-27 20:51:40 +0100 CET</v>
+      </c>
+      <c r="D161" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sortirDouche\danifae_1488.jpg</v>
+      </c>
+      <c r="E161" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sortirDouche</v>
+      </c>
+    </row>
+    <row r="162"/>
+    <row r="163">
+      <c r="A163">
+        <v>162</v>
+      </c>
+      <c r="B163" t="str">
+        <v>would-i-make-you-hard-if-i-sent-you-shower-nudes-boiq95qes1-1080x1440.jpg</v>
+      </c>
+      <c r="C163" t="str">
+        <v>2022-03-09 21:09:57.1381803 +0100 CET</v>
+      </c>
+      <c r="D163" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sortirDouche\would-i-make-you-hard-if-i-sent-you-shower-nudes-boiq95qes1-1080x1440.jpg</v>
+      </c>
+      <c r="E163" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\sortirDouche</v>
+      </c>
+    </row>
+    <row r="164"/>
+    <row r="165"/>
+    <row r="166"/>
+    <row r="167">
+      <c r="A167">
+        <v>166</v>
+      </c>
+      <c r="B167" t="str">
+        <v>95833571_001_173d.jpg</v>
+      </c>
+      <c r="C167" t="str">
+        <v>2022-03-30 21:33:14.8811013 +0200 CEST</v>
+      </c>
+      <c r="D167" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\towel\95833571_001_173d.jpg</v>
+      </c>
+      <c r="E167" t="str">
+        <v>F:\testBis\dl\Nouveau dossier\_Jeux\towel</v>
       </c>
     </row>
   </sheetData>

</xml_diff>